<commit_message>
Mediciones MOS max pot
</commit_message>
<xml_diff>
--- a/Mediciones/Libro1.xlsx
+++ b/Mediciones/Libro1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Mediciones</t>
   </si>
@@ -80,12 +80,6 @@
     <t>IL (Vd - VLaGND) (Hi res Zoom) ch2 = Vo ch1 = VLaGND</t>
   </si>
   <si>
-    <t>IL (Vd - VLaGND) (Normal)</t>
-  </si>
-  <si>
-    <t>IL (Vd - VLaGND) (High res)</t>
-  </si>
-  <si>
     <t>La 57 y 58 son raras cuando medimos el apagado hay unas oscilaciones por ahí (470R)</t>
   </si>
   <si>
@@ -123,6 +117,30 @@
   </si>
   <si>
     <t>Ig, Vgs y PWM (apagado) ch1 = PWM, ch3 = Vgs, math = Ig</t>
+  </si>
+  <si>
+    <t>dbpp</t>
+  </si>
+  <si>
+    <t>Máxima potencia</t>
+  </si>
+  <si>
+    <t>Puse un reóstato y fui bajando desde 100Ohm para hasta que el pico (normal, no la delta) de IL mida 100mV (o sea 1A)</t>
+  </si>
+  <si>
+    <t>Coincidentemente la fuente marcaba 0.74A, la Ix teórica era 0.75A</t>
+  </si>
+  <si>
+    <t>R = 61Ohm</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>IL (Vd - VLaGND) (Normal) ch3 = Vo math = IL</t>
+  </si>
+  <si>
+    <t>IL (Vd - VLaGND) (High res) ch3 = Vo math = IL</t>
   </si>
 </sst>
 </file>
@@ -324,7 +342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -341,6 +359,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -353,7 +373,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -637,7 +656,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -650,29 +669,29 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16">
+      <c r="B1" s="18">
         <v>100</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="16">
+      <c r="C1" s="19"/>
+      <c r="D1" s="18">
         <v>470</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="17">
-        <v>50</v>
-      </c>
-      <c r="I1" s="19"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="20"/>
+      <c r="H1" s="19">
+        <v>61</v>
+      </c>
+      <c r="I1" s="21"/>
       <c r="M1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1">
         <v>16</v>
@@ -692,8 +711,12 @@
       <c r="G2" s="2">
         <v>66</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="5"/>
+      <c r="H2" s="12">
+        <v>105</v>
+      </c>
+      <c r="I2" s="5">
+        <v>106</v>
+      </c>
       <c r="M2" t="s">
         <v>7</v>
       </c>
@@ -720,15 +743,19 @@
       <c r="G3" s="2">
         <v>68</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="5"/>
+      <c r="H3" s="12">
+        <v>107</v>
+      </c>
+      <c r="I3" s="5">
+        <v>108</v>
+      </c>
       <c r="M3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1">
         <v>9</v>
@@ -748,8 +775,12 @@
       <c r="G4" s="2">
         <v>70</v>
       </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="5"/>
+      <c r="H4" s="12">
+        <v>109</v>
+      </c>
+      <c r="I4" s="5">
+        <v>110</v>
+      </c>
       <c r="M4" t="s">
         <v>9</v>
       </c>
@@ -776,8 +807,12 @@
       <c r="G5" s="2">
         <v>72</v>
       </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="5"/>
+      <c r="H5" s="12">
+        <v>111</v>
+      </c>
+      <c r="I5" s="5">
+        <v>112</v>
+      </c>
       <c r="M5" t="s">
         <v>10</v>
       </c>
@@ -793,34 +828,38 @@
         <v>8</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G6" s="2"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="5"/>
+      <c r="H6" s="12">
+        <v>113</v>
+      </c>
+      <c r="I6" s="5">
+        <v>114</v>
+      </c>
       <c r="M6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="B7" s="12">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="C7" s="12">
-        <v>28</v>
+        <v>94</v>
       </c>
       <c r="D7" s="10">
-        <v>40</v>
+        <v>115</v>
       </c>
       <c r="E7" s="2">
-        <v>41</v>
+        <v>116</v>
       </c>
       <c r="F7" s="10">
         <v>75</v>
@@ -828,27 +867,31 @@
       <c r="G7" s="2">
         <v>76</v>
       </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="5"/>
+      <c r="H7" s="12">
+        <v>99</v>
+      </c>
+      <c r="I7" s="5">
+        <v>100</v>
+      </c>
       <c r="M7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="B8" s="12">
-        <v>25</v>
+        <v>95</v>
       </c>
       <c r="C8" s="12">
-        <v>26</v>
+        <v>96</v>
       </c>
       <c r="D8" s="10">
-        <v>38</v>
+        <v>117</v>
       </c>
       <c r="E8" s="2">
-        <v>39</v>
+        <v>118</v>
       </c>
       <c r="F8" s="10">
         <v>73</v>
@@ -856,8 +899,12 @@
       <c r="G8" s="2">
         <v>74</v>
       </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="5"/>
+      <c r="H8" s="12">
+        <v>101</v>
+      </c>
+      <c r="I8" s="5">
+        <v>102</v>
+      </c>
       <c r="M8" t="s">
         <v>13</v>
       </c>
@@ -866,8 +913,12 @@
       <c r="A9" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
+      <c r="B9" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>31</v>
+      </c>
       <c r="D9" s="10">
         <v>42</v>
       </c>
@@ -880,20 +931,31 @@
       <c r="G9" s="2">
         <v>78</v>
       </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="5"/>
+      <c r="H9" s="12">
+        <v>103</v>
+      </c>
+      <c r="I9" s="5">
+        <v>104</v>
+      </c>
+      <c r="J9" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
+        <v>28</v>
+      </c>
+      <c r="B10" s="12">
+        <v>97</v>
+      </c>
+      <c r="C10" s="12">
+        <v>98</v>
+      </c>
       <c r="D10" s="10">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="E10" s="2">
-        <v>47</v>
+        <v>121</v>
       </c>
       <c r="F10" s="10">
         <v>79</v>
@@ -901,8 +963,7 @@
       <c r="G10" s="2">
         <v>80</v>
       </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="5"/>
+      <c r="J10" s="17"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
@@ -922,8 +983,12 @@
       <c r="G11" s="2">
         <v>82</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="5"/>
+      <c r="H11" s="12">
+        <v>122</v>
+      </c>
+      <c r="I11" s="5">
+        <v>123</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
@@ -943,12 +1008,16 @@
       <c r="G12" s="2">
         <v>84</v>
       </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="5"/>
+      <c r="H12" s="12">
+        <v>124</v>
+      </c>
+      <c r="I12" s="5">
+        <v>125</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -969,7 +1038,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -985,10 +1054,10 @@
       <c r="G14" s="2">
         <v>88</v>
       </c>
-      <c r="H14" s="20"/>
+      <c r="H14" s="16"/>
       <c r="I14" s="5"/>
       <c r="J14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -1021,7 +1090,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B19">
         <v>61</v>
@@ -1030,12 +1099,12 @@
         <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -1046,10 +1115,30 @@
         <v>64</v>
       </c>
       <c r="D22" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24">
+        <v>99</v>
+      </c>
+      <c r="C24">
+        <v>100</v>
+      </c>
+      <c r="D24" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" t="s">
+        <v>34</v>
+      </c>
       <c r="H25" s="15"/>
     </row>
   </sheetData>

</xml_diff>